<commit_message>
Update UC diagram and matrix
</commit_message>
<xml_diff>
--- a/Matricos.xlsx
+++ b/Matricos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="98">
   <si>
     <t>UC1</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>FR54</t>
+  </si>
+  <si>
+    <t>UC20</t>
   </si>
 </sst>
 </file>
@@ -538,6 +541,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3360E5B-BDCB-4465-9C1E-88B12EF46913}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7886700" y="200025"/>
+          <a:ext cx="7210425" cy="6686550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -803,19 +872,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:W93"/>
+  <dimension ref="B1:W101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AO15" sqref="AO15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="26" width="5.140625" customWidth="1"/>
+    <col min="1" max="34" width="5.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -871,11 +940,14 @@
       <c r="T2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V2" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
@@ -899,9 +971,10 @@
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
-      <c r="U3" s="6"/>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U3" s="5"/>
+      <c r="V3" s="6"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
@@ -925,9 +998,10 @@
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
-      <c r="U4" s="6"/>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U4" s="5"/>
+      <c r="V4" s="6"/>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
@@ -951,9 +1025,10 @@
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
-      <c r="U5" s="6"/>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U5" s="5"/>
+      <c r="V5" s="6"/>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
@@ -977,9 +1052,10 @@
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
-      <c r="U6" s="6"/>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U6" s="5"/>
+      <c r="V6" s="6"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>23</v>
       </c>
@@ -1003,9 +1079,10 @@
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
-      <c r="U7" s="6"/>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U7" s="5"/>
+      <c r="V7" s="6"/>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
@@ -1029,9 +1106,10 @@
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
-      <c r="U8" s="6"/>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U8" s="5"/>
+      <c r="V8" s="6"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
@@ -1055,9 +1133,10 @@
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
-      <c r="U9" s="6"/>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U9" s="5"/>
+      <c r="V9" s="6"/>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>26</v>
       </c>
@@ -1081,9 +1160,10 @@
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
-      <c r="U10" s="6"/>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U10" s="5"/>
+      <c r="V10" s="6"/>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>27</v>
       </c>
@@ -1107,9 +1187,10 @@
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
-      <c r="U11" s="6"/>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U11" s="5"/>
+      <c r="V11" s="6"/>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>28</v>
       </c>
@@ -1133,9 +1214,10 @@
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
-      <c r="U12" s="6"/>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U12" s="5"/>
+      <c r="V12" s="6"/>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>29</v>
       </c>
@@ -1159,9 +1241,10 @@
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
-      <c r="U13" s="6"/>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U13" s="5"/>
+      <c r="V13" s="6"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>30</v>
       </c>
@@ -1185,9 +1268,10 @@
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
-      <c r="U14" s="6"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U14" s="5"/>
+      <c r="V14" s="6"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
@@ -1211,9 +1295,10 @@
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
       <c r="T15" s="5"/>
-      <c r="U15" s="6"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U15" s="5"/>
+      <c r="V15" s="6"/>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>32</v>
       </c>
@@ -1237,9 +1322,10 @@
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
-      <c r="U16" s="6"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U16" s="5"/>
+      <c r="V16" s="6"/>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>33</v>
       </c>
@@ -1263,9 +1349,10 @@
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
-      <c r="U17" s="6"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U17" s="5"/>
+      <c r="V17" s="6"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>34</v>
       </c>
@@ -1289,9 +1376,10 @@
       </c>
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
-      <c r="U18" s="6"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U18" s="5"/>
+      <c r="V18" s="6"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>35</v>
       </c>
@@ -1315,9 +1403,10 @@
         <v>52</v>
       </c>
       <c r="T19" s="5"/>
-      <c r="U19" s="6"/>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U19" s="5"/>
+      <c r="V19" s="6"/>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>36</v>
       </c>
@@ -1341,9 +1430,10 @@
       <c r="T20" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="U20" s="6"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U20" s="5"/>
+      <c r="V20" s="6"/>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>37</v>
       </c>
@@ -1365,11 +1455,12 @@
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
-      <c r="U21" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U21" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="V21" s="6"/>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>38</v>
       </c>
@@ -1395,9 +1486,10 @@
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
-      <c r="U22" s="6"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U22" s="5"/>
+      <c r="V22" s="6"/>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>39</v>
       </c>
@@ -1423,9 +1515,10 @@
       <c r="R23" s="5"/>
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
-      <c r="U23" s="6"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U23" s="5"/>
+      <c r="V23" s="6"/>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>40</v>
       </c>
@@ -1449,9 +1542,10 @@
       <c r="R24" s="5"/>
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
-      <c r="U24" s="6"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U24" s="5"/>
+      <c r="V24" s="6"/>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>41</v>
       </c>
@@ -1475,9 +1569,10 @@
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
-      <c r="U25" s="6"/>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U25" s="5"/>
+      <c r="V25" s="6"/>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>42</v>
       </c>
@@ -1501,9 +1596,10 @@
       <c r="R26" s="5"/>
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
-      <c r="U26" s="6"/>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U26" s="5"/>
+      <c r="V26" s="6"/>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>43</v>
       </c>
@@ -1527,9 +1623,10 @@
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
-      <c r="U27" s="6"/>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U27" s="5"/>
+      <c r="V27" s="6"/>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>44</v>
       </c>
@@ -1553,9 +1650,10 @@
       <c r="R28" s="5"/>
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
-      <c r="U28" s="6"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U28" s="5"/>
+      <c r="V28" s="6"/>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>45</v>
       </c>
@@ -1579,9 +1677,10 @@
       <c r="R29" s="5"/>
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
-      <c r="U29" s="6"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U29" s="5"/>
+      <c r="V29" s="6"/>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>46</v>
       </c>
@@ -1607,9 +1706,10 @@
       <c r="R30" s="5"/>
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
-      <c r="U30" s="6"/>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U30" s="5"/>
+      <c r="V30" s="6"/>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>47</v>
       </c>
@@ -1633,9 +1733,10 @@
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
       <c r="T31" s="5"/>
-      <c r="U31" s="6"/>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U31" s="5"/>
+      <c r="V31" s="6"/>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>48</v>
       </c>
@@ -1661,7 +1762,8 @@
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
-      <c r="U32" s="6"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="6"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
@@ -1689,18 +1791,17 @@
       <c r="R33" s="5"/>
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
-      <c r="U33" s="6"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="6"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
-        <v>50</v>
+      <c r="B34" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
-      <c r="F34" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -1715,323 +1816,140 @@
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
-      <c r="U34" s="6"/>
-    </row>
-    <row r="35" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="7" t="s">
+      <c r="U34" s="5"/>
+      <c r="V34" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="6"/>
+    </row>
+    <row r="36" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="9"/>
-    </row>
-    <row r="36" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-      <c r="C37" s="2" t="s">
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="9"/>
+    </row>
+    <row r="44" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
+      <c r="C45" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H45" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="I45" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="J45" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="K37" s="2" t="s">
+      <c r="K45" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="L37" s="2" t="s">
+      <c r="L45" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M37" s="2" t="s">
+      <c r="M45" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N37" s="2" t="s">
+      <c r="N45" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O37" s="2" t="s">
+      <c r="O45" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P37" s="2" t="s">
+      <c r="P45" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Q37" s="2" t="s">
+      <c r="Q45" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="R37" s="2" t="s">
+      <c r="R45" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="S37" s="2" t="s">
+      <c r="S45" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="T37" s="2" t="s">
+      <c r="T45" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="U37" s="2" t="s">
+      <c r="U45" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="V37" s="2" t="s">
+      <c r="V45" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="W37" s="3" t="s">
+      <c r="W45" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B38" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="5"/>
-      <c r="R38" s="5"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="5"/>
-      <c r="U38" s="5"/>
-      <c r="V38" s="5"/>
-      <c r="W38" s="6"/>
-    </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B39" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
-      <c r="U39" s="5"/>
-      <c r="V39" s="5"/>
-      <c r="W39" s="6"/>
-    </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B40" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="5"/>
-      <c r="U40" s="5"/>
-      <c r="V40" s="5"/>
-      <c r="W40" s="6"/>
-    </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B41" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
-      <c r="U41" s="5"/>
-      <c r="V41" s="5"/>
-      <c r="W41" s="6"/>
-    </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B42" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
-      <c r="U42" s="5"/>
-      <c r="V42" s="5"/>
-      <c r="W42" s="6"/>
-    </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B43" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="5"/>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="5"/>
-      <c r="U43" s="5"/>
-      <c r="V43" s="5"/>
-      <c r="W43" s="6"/>
-    </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B44" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="5"/>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="5"/>
-      <c r="R44" s="5"/>
-      <c r="S44" s="5"/>
-      <c r="T44" s="5"/>
-      <c r="U44" s="5"/>
-      <c r="V44" s="5"/>
-      <c r="W44" s="6"/>
-    </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B45" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="5"/>
-      <c r="U45" s="5"/>
-      <c r="V45" s="5"/>
-      <c r="W45" s="6"/>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B46" s="10" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="D46" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -2054,12 +1972,14 @@
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
+      <c r="F47" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -2080,9 +2000,11 @@
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -2106,7 +2028,7 @@
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B49" s="10" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>52</v>
@@ -2134,11 +2056,9 @@
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -2162,7 +2082,7 @@
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -2188,7 +2108,7 @@
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B52" s="10" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -2214,16 +2134,14 @@
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B53" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
-      <c r="H53" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
@@ -2242,15 +2160,13 @@
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
-      <c r="G54" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="G54" s="5"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
@@ -2270,15 +2186,13 @@
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B55" s="10" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
-      <c r="G55" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="G55" s="5"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
@@ -2298,7 +2212,7 @@
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -2324,9 +2238,11 @@
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C57" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
@@ -2350,9 +2266,11 @@
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C58" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
@@ -2376,7 +2294,7 @@
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
@@ -2402,7 +2320,7 @@
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -2428,14 +2346,16 @@
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B61" s="10" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
+      <c r="H61" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
@@ -2454,13 +2374,15 @@
     </row>
     <row r="62" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B62" s="10" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
+      <c r="G62" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
@@ -2480,13 +2402,15 @@
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B63" s="10" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
+      <c r="G63" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
@@ -2506,7 +2430,7 @@
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B64" s="10" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -2532,7 +2456,7 @@
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B65" s="10" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -2558,7 +2482,7 @@
     </row>
     <row r="66" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -2584,7 +2508,7 @@
     </row>
     <row r="67" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B67" s="10" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -2610,7 +2534,7 @@
     </row>
     <row r="68" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B68" s="10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -2636,7 +2560,7 @@
     </row>
     <row r="69" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B69" s="10" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -2662,7 +2586,7 @@
     </row>
     <row r="70" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B70" s="10" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -2688,7 +2612,7 @@
     </row>
     <row r="71" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B71" s="10" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -2714,7 +2638,7 @@
     </row>
     <row r="72" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B72" s="10" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -2740,11 +2664,9 @@
     </row>
     <row r="73" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B73" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
@@ -2768,14 +2690,12 @@
     </row>
     <row r="74" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B74" s="10" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
-      <c r="F74" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="F74" s="5"/>
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
@@ -2796,11 +2716,9 @@
     </row>
     <row r="75" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B75" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
@@ -2824,7 +2742,7 @@
     </row>
     <row r="76" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B76" s="10" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -2850,12 +2768,10 @@
     </row>
     <row r="77" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B77" s="10" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="C77" s="5"/>
-      <c r="D77" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="D77" s="5"/>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
       <c r="G77" s="5"/>
@@ -2878,12 +2794,10 @@
     </row>
     <row r="78" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B78" s="10" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="C78" s="5"/>
-      <c r="D78" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
       <c r="G78" s="5"/>
@@ -2906,12 +2820,10 @@
     </row>
     <row r="79" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B79" s="10" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="C79" s="5"/>
-      <c r="D79" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="D79" s="5"/>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
       <c r="G79" s="5"/>
@@ -2934,14 +2846,12 @@
     </row>
     <row r="80" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B80" s="10" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
-      <c r="F80" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="F80" s="5"/>
       <c r="G80" s="5"/>
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
@@ -2962,14 +2872,14 @@
     </row>
     <row r="81" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B81" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C81" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
-      <c r="F81" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="F81" s="5"/>
       <c r="G81" s="5"/>
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
@@ -2990,14 +2900,14 @@
     </row>
     <row r="82" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B82" s="10" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
-      <c r="E82" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
@@ -3018,9 +2928,11 @@
     </row>
     <row r="83" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B83" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C83" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
@@ -3044,7 +2956,7 @@
     </row>
     <row r="84" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B84" s="10" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
@@ -3070,10 +2982,12 @@
     </row>
     <row r="85" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B85" s="10" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
+      <c r="D85" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
       <c r="G85" s="5"/>
@@ -3096,13 +3010,13 @@
     </row>
     <row r="86" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B86" s="10" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="D86" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E86" s="5"/>
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
@@ -3124,13 +3038,13 @@
     </row>
     <row r="87" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B87" s="10" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="C87" s="5"/>
-      <c r="D87" s="5"/>
-      <c r="E87" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="D87" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E87" s="5"/>
       <c r="F87" s="5"/>
       <c r="G87" s="5"/>
       <c r="H87" s="5"/>
@@ -3152,12 +3066,14 @@
     </row>
     <row r="88" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B88" s="10" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
+      <c r="F88" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="G88" s="5"/>
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
@@ -3178,12 +3094,14 @@
     </row>
     <row r="89" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B89" s="10" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
+      <c r="F89" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="G89" s="5"/>
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
@@ -3204,11 +3122,13 @@
     </row>
     <row r="90" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B90" s="10" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
+      <c r="E90" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
@@ -3230,7 +3150,7 @@
     </row>
     <row r="91" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B91" s="10" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
@@ -3256,7 +3176,7 @@
     </row>
     <row r="92" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B92" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
@@ -3280,34 +3200,247 @@
       <c r="V92" s="5"/>
       <c r="W92" s="6"/>
     </row>
-    <row r="93" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="11" t="s">
+    <row r="93" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B93" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5"/>
+      <c r="I93" s="5"/>
+      <c r="J93" s="5"/>
+      <c r="K93" s="5"/>
+      <c r="L93" s="5"/>
+      <c r="M93" s="5"/>
+      <c r="N93" s="5"/>
+      <c r="O93" s="5"/>
+      <c r="P93" s="5"/>
+      <c r="Q93" s="5"/>
+      <c r="R93" s="5"/>
+      <c r="S93" s="5"/>
+      <c r="T93" s="5"/>
+      <c r="U93" s="5"/>
+      <c r="V93" s="5"/>
+      <c r="W93" s="6"/>
+    </row>
+    <row r="94" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B94" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
+      <c r="I94" s="5"/>
+      <c r="J94" s="5"/>
+      <c r="K94" s="5"/>
+      <c r="L94" s="5"/>
+      <c r="M94" s="5"/>
+      <c r="N94" s="5"/>
+      <c r="O94" s="5"/>
+      <c r="P94" s="5"/>
+      <c r="Q94" s="5"/>
+      <c r="R94" s="5"/>
+      <c r="S94" s="5"/>
+      <c r="T94" s="5"/>
+      <c r="U94" s="5"/>
+      <c r="V94" s="5"/>
+      <c r="W94" s="6"/>
+    </row>
+    <row r="95" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B95" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="5"/>
+      <c r="I95" s="5"/>
+      <c r="J95" s="5"/>
+      <c r="K95" s="5"/>
+      <c r="L95" s="5"/>
+      <c r="M95" s="5"/>
+      <c r="N95" s="5"/>
+      <c r="O95" s="5"/>
+      <c r="P95" s="5"/>
+      <c r="Q95" s="5"/>
+      <c r="R95" s="5"/>
+      <c r="S95" s="5"/>
+      <c r="T95" s="5"/>
+      <c r="U95" s="5"/>
+      <c r="V95" s="5"/>
+      <c r="W95" s="6"/>
+    </row>
+    <row r="96" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B96" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="5"/>
+      <c r="I96" s="5"/>
+      <c r="J96" s="5"/>
+      <c r="K96" s="5"/>
+      <c r="L96" s="5"/>
+      <c r="M96" s="5"/>
+      <c r="N96" s="5"/>
+      <c r="O96" s="5"/>
+      <c r="P96" s="5"/>
+      <c r="Q96" s="5"/>
+      <c r="R96" s="5"/>
+      <c r="S96" s="5"/>
+      <c r="T96" s="5"/>
+      <c r="U96" s="5"/>
+      <c r="V96" s="5"/>
+      <c r="W96" s="6"/>
+    </row>
+    <row r="97" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B97" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="5"/>
+      <c r="I97" s="5"/>
+      <c r="J97" s="5"/>
+      <c r="K97" s="5"/>
+      <c r="L97" s="5"/>
+      <c r="M97" s="5"/>
+      <c r="N97" s="5"/>
+      <c r="O97" s="5"/>
+      <c r="P97" s="5"/>
+      <c r="Q97" s="5"/>
+      <c r="R97" s="5"/>
+      <c r="S97" s="5"/>
+      <c r="T97" s="5"/>
+      <c r="U97" s="5"/>
+      <c r="V97" s="5"/>
+      <c r="W97" s="6"/>
+    </row>
+    <row r="98" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B98" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
+      <c r="I98" s="5"/>
+      <c r="J98" s="5"/>
+      <c r="K98" s="5"/>
+      <c r="L98" s="5"/>
+      <c r="M98" s="5"/>
+      <c r="N98" s="5"/>
+      <c r="O98" s="5"/>
+      <c r="P98" s="5"/>
+      <c r="Q98" s="5"/>
+      <c r="R98" s="5"/>
+      <c r="S98" s="5"/>
+      <c r="T98" s="5"/>
+      <c r="U98" s="5"/>
+      <c r="V98" s="5"/>
+      <c r="W98" s="6"/>
+    </row>
+    <row r="99" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B99" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5"/>
+      <c r="H99" s="5"/>
+      <c r="I99" s="5"/>
+      <c r="J99" s="5"/>
+      <c r="K99" s="5"/>
+      <c r="L99" s="5"/>
+      <c r="M99" s="5"/>
+      <c r="N99" s="5"/>
+      <c r="O99" s="5"/>
+      <c r="P99" s="5"/>
+      <c r="Q99" s="5"/>
+      <c r="R99" s="5"/>
+      <c r="S99" s="5"/>
+      <c r="T99" s="5"/>
+      <c r="U99" s="5"/>
+      <c r="V99" s="5"/>
+      <c r="W99" s="6"/>
+    </row>
+    <row r="100" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B100" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+      <c r="I100" s="5"/>
+      <c r="J100" s="5"/>
+      <c r="K100" s="5"/>
+      <c r="L100" s="5"/>
+      <c r="M100" s="5"/>
+      <c r="N100" s="5"/>
+      <c r="O100" s="5"/>
+      <c r="P100" s="5"/>
+      <c r="Q100" s="5"/>
+      <c r="R100" s="5"/>
+      <c r="S100" s="5"/>
+      <c r="T100" s="5"/>
+      <c r="U100" s="5"/>
+      <c r="V100" s="5"/>
+      <c r="W100" s="6"/>
+    </row>
+    <row r="101" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C93" s="8"/>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="8"/>
-      <c r="G93" s="8"/>
-      <c r="H93" s="8"/>
-      <c r="I93" s="8"/>
-      <c r="J93" s="8"/>
-      <c r="K93" s="8"/>
-      <c r="L93" s="8"/>
-      <c r="M93" s="8"/>
-      <c r="N93" s="8"/>
-      <c r="O93" s="8"/>
-      <c r="P93" s="8"/>
-      <c r="Q93" s="8"/>
-      <c r="R93" s="8"/>
-      <c r="S93" s="8"/>
-      <c r="T93" s="8"/>
-      <c r="U93" s="8"/>
-      <c r="V93" s="8"/>
-      <c r="W93" s="9"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="8"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="8"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="8"/>
+      <c r="I101" s="8"/>
+      <c r="J101" s="8"/>
+      <c r="K101" s="8"/>
+      <c r="L101" s="8"/>
+      <c r="M101" s="8"/>
+      <c r="N101" s="8"/>
+      <c r="O101" s="8"/>
+      <c r="P101" s="8"/>
+      <c r="Q101" s="8"/>
+      <c r="R101" s="8"/>
+      <c r="S101" s="8"/>
+      <c r="T101" s="8"/>
+      <c r="U101" s="8"/>
+      <c r="V101" s="8"/>
+      <c r="W101" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add screenshots, entity matrix, entity table and some other minor fixes
</commit_message>
<xml_diff>
--- a/Matricos.xlsx
+++ b/Matricos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="81">
   <si>
     <t>UC1</t>
   </si>
@@ -243,54 +243,6 @@
     <t>G9</t>
   </si>
   <si>
-    <t>FR20</t>
-  </si>
-  <si>
-    <t>FR21</t>
-  </si>
-  <si>
-    <t>FR22</t>
-  </si>
-  <si>
-    <t>FR23</t>
-  </si>
-  <si>
-    <t>FR24</t>
-  </si>
-  <si>
-    <t>FR25</t>
-  </si>
-  <si>
-    <t>FR26</t>
-  </si>
-  <si>
-    <t>FR27</t>
-  </si>
-  <si>
-    <t>FR28</t>
-  </si>
-  <si>
-    <t>FR29</t>
-  </si>
-  <si>
-    <t>FR30</t>
-  </si>
-  <si>
-    <t>FR31</t>
-  </si>
-  <si>
-    <t>FR32</t>
-  </si>
-  <si>
-    <t>FR33</t>
-  </si>
-  <si>
-    <t>FR34</t>
-  </si>
-  <si>
-    <t>FR35</t>
-  </si>
-  <si>
     <t>FR36</t>
   </si>
   <si>
@@ -307,9 +259,6 @@
   </si>
   <si>
     <t>FR53</t>
-  </si>
-  <si>
-    <t>FR54</t>
   </si>
   <si>
     <t>UC20</t>
@@ -547,23 +496,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3360E5B-BDCB-4465-9C1E-88B12EF46913}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9C7957E-5114-4AC0-B33A-9427D8594DD3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -586,8 +535,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7886700" y="200025"/>
-          <a:ext cx="7210425" cy="6686550"/>
+          <a:off x="8229600" y="7077075"/>
+          <a:ext cx="7553325" cy="6496050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -872,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:W101"/>
+  <dimension ref="B1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AO15" sqref="AO15"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="AP54" sqref="AP54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,7 +893,7 @@
         <v>18</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
@@ -1796,7 +1745,7 @@
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1875,89 +1824,299 @@
       <c r="U36" s="8"/>
       <c r="V36" s="9"/>
     </row>
-    <row r="44" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+      <c r="C38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="S38" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T38" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="U38" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="V38" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="W38" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B39" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5"/>
+      <c r="S39" s="5"/>
+      <c r="T39" s="5"/>
+      <c r="U39" s="5"/>
+      <c r="V39" s="5"/>
+      <c r="W39" s="6"/>
+    </row>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B40" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="5"/>
+      <c r="U40" s="5"/>
+      <c r="V40" s="5"/>
+      <c r="W40" s="6"/>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B41" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="V41" s="5"/>
+      <c r="W41" s="6"/>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B42" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="V42" s="5"/>
+      <c r="W42" s="6"/>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B43" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="5"/>
+      <c r="S43" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="T43" s="5"/>
+      <c r="U43" s="5"/>
+      <c r="V43" s="5"/>
+      <c r="W43" s="6"/>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B44" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="5"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="5"/>
+      <c r="U44" s="5"/>
+      <c r="V44" s="5"/>
+      <c r="W44" s="6"/>
+    </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
-      <c r="C45" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="L45" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="N45" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="O45" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="P45" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q45" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R45" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="S45" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="T45" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="U45" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="V45" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W45" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="B45" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
+      <c r="U45" s="5"/>
+      <c r="V45" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="W45" s="6"/>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B46" s="10" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C46" s="5"/>
-      <c r="D46" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
+      <c r="K46" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L46" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
@@ -1967,25 +2126,29 @@
       <c r="S46" s="5"/>
       <c r="T46" s="5"/>
       <c r="U46" s="5"/>
-      <c r="V46" s="5"/>
+      <c r="V46" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="W46" s="6"/>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
-      <c r="F47" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="F47" s="5"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
+      <c r="K47" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L47" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="M47" s="5"/>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
@@ -1995,16 +2158,16 @@
       <c r="S47" s="5"/>
       <c r="T47" s="5"/>
       <c r="U47" s="5"/>
-      <c r="V47" s="5"/>
+      <c r="V47" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="W47" s="6"/>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -2012,7 +2175,9 @@
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
+      <c r="K48" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
@@ -2023,12 +2188,14 @@
       <c r="S48" s="5"/>
       <c r="T48" s="5"/>
       <c r="U48" s="5"/>
-      <c r="V48" s="5"/>
+      <c r="V48" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="W48" s="6"/>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B49" s="10" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>52</v>
@@ -2050,15 +2217,21 @@
       <c r="R49" s="5"/>
       <c r="S49" s="5"/>
       <c r="T49" s="5"/>
-      <c r="U49" s="5"/>
+      <c r="U49" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="V49" s="5"/>
-      <c r="W49" s="6"/>
+      <c r="W49" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -2078,11 +2251,13 @@
       <c r="T50" s="5"/>
       <c r="U50" s="5"/>
       <c r="V50" s="5"/>
-      <c r="W50" s="6"/>
+      <c r="W50" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -2091,11 +2266,19 @@
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
+      <c r="J51" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
+      <c r="M51" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N51" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
       <c r="Q51" s="5"/>
@@ -2108,14 +2291,16 @@
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B52" s="10" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
+      <c r="H52" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
@@ -2134,13 +2319,15 @@
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B53" s="10" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
+      <c r="G53" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
@@ -2153,20 +2340,24 @@
       <c r="Q53" s="5"/>
       <c r="R53" s="5"/>
       <c r="S53" s="5"/>
-      <c r="T53" s="5"/>
+      <c r="T53" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="U53" s="5"/>
       <c r="V53" s="5"/>
       <c r="W53" s="6"/>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
+      <c r="G54" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
@@ -2180,15 +2371,19 @@
       <c r="R54" s="5"/>
       <c r="S54" s="5"/>
       <c r="T54" s="5"/>
-      <c r="U54" s="5"/>
+      <c r="U54" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="V54" s="5"/>
       <c r="W54" s="6"/>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B55" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C55" s="5"/>
+        <v>74</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
@@ -2200,7 +2395,9 @@
       <c r="L55" s="5"/>
       <c r="M55" s="5"/>
       <c r="N55" s="5"/>
-      <c r="O55" s="5"/>
+      <c r="O55" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="P55" s="5"/>
       <c r="Q55" s="5"/>
       <c r="R55" s="5"/>
@@ -2212,12 +2409,14 @@
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
+      <c r="F56" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
@@ -2238,7 +2437,7 @@
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>52</v>
@@ -2266,19 +2465,21 @@
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
-      <c r="J58" s="5"/>
-      <c r="K58" s="5"/>
+      <c r="J58" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K58" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="L58" s="5"/>
       <c r="M58" s="5"/>
       <c r="N58" s="5"/>
@@ -2294,10 +2495,12 @@
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="D59" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
@@ -2320,10 +2523,12 @@
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+      <c r="D60" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
@@ -2346,16 +2551,16 @@
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B61" s="10" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+      <c r="D61" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
-      <c r="H61" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
@@ -2374,15 +2579,15 @@
     </row>
     <row r="62" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B62" s="10" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="F62" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G62" s="5"/>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
@@ -2391,7 +2596,9 @@
       <c r="M62" s="5"/>
       <c r="N62" s="5"/>
       <c r="O62" s="5"/>
-      <c r="P62" s="5"/>
+      <c r="P62" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="Q62" s="5"/>
       <c r="R62" s="5"/>
       <c r="S62" s="5"/>
@@ -2402,15 +2609,15 @@
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B63" s="10" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="F63" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G63" s="5"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
@@ -2419,7 +2626,9 @@
       <c r="M63" s="5"/>
       <c r="N63" s="5"/>
       <c r="O63" s="5"/>
-      <c r="P63" s="5"/>
+      <c r="P63" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="Q63" s="5"/>
       <c r="R63" s="5"/>
       <c r="S63" s="5"/>
@@ -2430,17 +2639,23 @@
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B64" s="10" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
+      <c r="E64" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
+      <c r="J64" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K64" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="L64" s="5"/>
       <c r="M64" s="5"/>
       <c r="N64" s="5"/>
@@ -2451,12 +2666,14 @@
       <c r="S64" s="5"/>
       <c r="T64" s="5"/>
       <c r="U64" s="5"/>
-      <c r="V64" s="5"/>
+      <c r="V64" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="W64" s="6"/>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B65" s="10" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -2466,8 +2683,12 @@
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
-      <c r="K65" s="5"/>
-      <c r="L65" s="5"/>
+      <c r="K65" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L65" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="M65" s="5"/>
       <c r="N65" s="5"/>
       <c r="O65" s="5"/>
@@ -2482,7 +2703,7 @@
     </row>
     <row r="66" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -2492,8 +2713,12 @@
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
-      <c r="K66" s="5"/>
-      <c r="L66" s="5"/>
+      <c r="K66" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L66" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="M66" s="5"/>
       <c r="N66" s="5"/>
       <c r="O66" s="5"/>
@@ -2508,7 +2733,7 @@
     </row>
     <row r="67" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B67" s="10" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -2518,8 +2743,12 @@
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="5"/>
+      <c r="K67" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L67" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="M67" s="5"/>
       <c r="N67" s="5"/>
       <c r="O67" s="5"/>
@@ -2534,11 +2763,13 @@
     </row>
     <row r="68" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B68" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
+      <c r="E68" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
@@ -2560,11 +2791,13 @@
     </row>
     <row r="69" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B69" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
+      <c r="E69" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
@@ -2586,7 +2819,7 @@
     </row>
     <row r="70" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B70" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -2594,7 +2827,9 @@
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
+      <c r="I70" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="J70" s="5"/>
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
@@ -2604,839 +2839,43 @@
       <c r="P70" s="5"/>
       <c r="Q70" s="5"/>
       <c r="R70" s="5"/>
-      <c r="S70" s="5"/>
+      <c r="S70" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="T70" s="5"/>
       <c r="U70" s="5"/>
       <c r="V70" s="5"/>
       <c r="W70" s="6"/>
     </row>
-    <row r="71" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B71" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
-      <c r="J71" s="5"/>
-      <c r="K71" s="5"/>
-      <c r="L71" s="5"/>
-      <c r="M71" s="5"/>
-      <c r="N71" s="5"/>
-      <c r="O71" s="5"/>
-      <c r="P71" s="5"/>
-      <c r="Q71" s="5"/>
-      <c r="R71" s="5"/>
-      <c r="S71" s="5"/>
-      <c r="T71" s="5"/>
-      <c r="U71" s="5"/>
-      <c r="V71" s="5"/>
-      <c r="W71" s="6"/>
-    </row>
-    <row r="72" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B72" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
-      <c r="I72" s="5"/>
-      <c r="J72" s="5"/>
-      <c r="K72" s="5"/>
-      <c r="L72" s="5"/>
-      <c r="M72" s="5"/>
-      <c r="N72" s="5"/>
-      <c r="O72" s="5"/>
-      <c r="P72" s="5"/>
-      <c r="Q72" s="5"/>
-      <c r="R72" s="5"/>
-      <c r="S72" s="5"/>
-      <c r="T72" s="5"/>
-      <c r="U72" s="5"/>
-      <c r="V72" s="5"/>
-      <c r="W72" s="6"/>
-    </row>
-    <row r="73" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B73" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
-      <c r="J73" s="5"/>
-      <c r="K73" s="5"/>
-      <c r="L73" s="5"/>
-      <c r="M73" s="5"/>
-      <c r="N73" s="5"/>
-      <c r="O73" s="5"/>
-      <c r="P73" s="5"/>
-      <c r="Q73" s="5"/>
-      <c r="R73" s="5"/>
-      <c r="S73" s="5"/>
-      <c r="T73" s="5"/>
-      <c r="U73" s="5"/>
-      <c r="V73" s="5"/>
-      <c r="W73" s="6"/>
-    </row>
-    <row r="74" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B74" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="5"/>
-      <c r="M74" s="5"/>
-      <c r="N74" s="5"/>
-      <c r="O74" s="5"/>
-      <c r="P74" s="5"/>
-      <c r="Q74" s="5"/>
-      <c r="R74" s="5"/>
-      <c r="S74" s="5"/>
-      <c r="T74" s="5"/>
-      <c r="U74" s="5"/>
-      <c r="V74" s="5"/>
-      <c r="W74" s="6"/>
-    </row>
-    <row r="75" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B75" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
-      <c r="J75" s="5"/>
-      <c r="K75" s="5"/>
-      <c r="L75" s="5"/>
-      <c r="M75" s="5"/>
-      <c r="N75" s="5"/>
-      <c r="O75" s="5"/>
-      <c r="P75" s="5"/>
-      <c r="Q75" s="5"/>
-      <c r="R75" s="5"/>
-      <c r="S75" s="5"/>
-      <c r="T75" s="5"/>
-      <c r="U75" s="5"/>
-      <c r="V75" s="5"/>
-      <c r="W75" s="6"/>
-    </row>
-    <row r="76" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B76" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
-      <c r="J76" s="5"/>
-      <c r="K76" s="5"/>
-      <c r="L76" s="5"/>
-      <c r="M76" s="5"/>
-      <c r="N76" s="5"/>
-      <c r="O76" s="5"/>
-      <c r="P76" s="5"/>
-      <c r="Q76" s="5"/>
-      <c r="R76" s="5"/>
-      <c r="S76" s="5"/>
-      <c r="T76" s="5"/>
-      <c r="U76" s="5"/>
-      <c r="V76" s="5"/>
-      <c r="W76" s="6"/>
-    </row>
-    <row r="77" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B77" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
-      <c r="I77" s="5"/>
-      <c r="J77" s="5"/>
-      <c r="K77" s="5"/>
-      <c r="L77" s="5"/>
-      <c r="M77" s="5"/>
-      <c r="N77" s="5"/>
-      <c r="O77" s="5"/>
-      <c r="P77" s="5"/>
-      <c r="Q77" s="5"/>
-      <c r="R77" s="5"/>
-      <c r="S77" s="5"/>
-      <c r="T77" s="5"/>
-      <c r="U77" s="5"/>
-      <c r="V77" s="5"/>
-      <c r="W77" s="6"/>
-    </row>
-    <row r="78" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B78" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
-      <c r="J78" s="5"/>
-      <c r="K78" s="5"/>
-      <c r="L78" s="5"/>
-      <c r="M78" s="5"/>
-      <c r="N78" s="5"/>
-      <c r="O78" s="5"/>
-      <c r="P78" s="5"/>
-      <c r="Q78" s="5"/>
-      <c r="R78" s="5"/>
-      <c r="S78" s="5"/>
-      <c r="T78" s="5"/>
-      <c r="U78" s="5"/>
-      <c r="V78" s="5"/>
-      <c r="W78" s="6"/>
-    </row>
-    <row r="79" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B79" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="5"/>
-      <c r="J79" s="5"/>
-      <c r="K79" s="5"/>
-      <c r="L79" s="5"/>
-      <c r="M79" s="5"/>
-      <c r="N79" s="5"/>
-      <c r="O79" s="5"/>
-      <c r="P79" s="5"/>
-      <c r="Q79" s="5"/>
-      <c r="R79" s="5"/>
-      <c r="S79" s="5"/>
-      <c r="T79" s="5"/>
-      <c r="U79" s="5"/>
-      <c r="V79" s="5"/>
-      <c r="W79" s="6"/>
-    </row>
-    <row r="80" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B80" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5"/>
-      <c r="I80" s="5"/>
-      <c r="J80" s="5"/>
-      <c r="K80" s="5"/>
-      <c r="L80" s="5"/>
-      <c r="M80" s="5"/>
-      <c r="N80" s="5"/>
-      <c r="O80" s="5"/>
-      <c r="P80" s="5"/>
-      <c r="Q80" s="5"/>
-      <c r="R80" s="5"/>
-      <c r="S80" s="5"/>
-      <c r="T80" s="5"/>
-      <c r="U80" s="5"/>
-      <c r="V80" s="5"/>
-      <c r="W80" s="6"/>
-    </row>
-    <row r="81" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B81" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="5"/>
-      <c r="H81" s="5"/>
-      <c r="I81" s="5"/>
-      <c r="J81" s="5"/>
-      <c r="K81" s="5"/>
-      <c r="L81" s="5"/>
-      <c r="M81" s="5"/>
-      <c r="N81" s="5"/>
-      <c r="O81" s="5"/>
-      <c r="P81" s="5"/>
-      <c r="Q81" s="5"/>
-      <c r="R81" s="5"/>
-      <c r="S81" s="5"/>
-      <c r="T81" s="5"/>
-      <c r="U81" s="5"/>
-      <c r="V81" s="5"/>
-      <c r="W81" s="6"/>
-    </row>
-    <row r="82" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B82" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G82" s="5"/>
-      <c r="H82" s="5"/>
-      <c r="I82" s="5"/>
-      <c r="J82" s="5"/>
-      <c r="K82" s="5"/>
-      <c r="L82" s="5"/>
-      <c r="M82" s="5"/>
-      <c r="N82" s="5"/>
-      <c r="O82" s="5"/>
-      <c r="P82" s="5"/>
-      <c r="Q82" s="5"/>
-      <c r="R82" s="5"/>
-      <c r="S82" s="5"/>
-      <c r="T82" s="5"/>
-      <c r="U82" s="5"/>
-      <c r="V82" s="5"/>
-      <c r="W82" s="6"/>
-    </row>
-    <row r="83" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B83" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="5"/>
-      <c r="H83" s="5"/>
-      <c r="I83" s="5"/>
-      <c r="J83" s="5"/>
-      <c r="K83" s="5"/>
-      <c r="L83" s="5"/>
-      <c r="M83" s="5"/>
-      <c r="N83" s="5"/>
-      <c r="O83" s="5"/>
-      <c r="P83" s="5"/>
-      <c r="Q83" s="5"/>
-      <c r="R83" s="5"/>
-      <c r="S83" s="5"/>
-      <c r="T83" s="5"/>
-      <c r="U83" s="5"/>
-      <c r="V83" s="5"/>
-      <c r="W83" s="6"/>
-    </row>
-    <row r="84" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B84" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="5"/>
-      <c r="H84" s="5"/>
-      <c r="I84" s="5"/>
-      <c r="J84" s="5"/>
-      <c r="K84" s="5"/>
-      <c r="L84" s="5"/>
-      <c r="M84" s="5"/>
-      <c r="N84" s="5"/>
-      <c r="O84" s="5"/>
-      <c r="P84" s="5"/>
-      <c r="Q84" s="5"/>
-      <c r="R84" s="5"/>
-      <c r="S84" s="5"/>
-      <c r="T84" s="5"/>
-      <c r="U84" s="5"/>
-      <c r="V84" s="5"/>
-      <c r="W84" s="6"/>
-    </row>
-    <row r="85" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B85" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E85" s="5"/>
-      <c r="F85" s="5"/>
-      <c r="G85" s="5"/>
-      <c r="H85" s="5"/>
-      <c r="I85" s="5"/>
-      <c r="J85" s="5"/>
-      <c r="K85" s="5"/>
-      <c r="L85" s="5"/>
-      <c r="M85" s="5"/>
-      <c r="N85" s="5"/>
-      <c r="O85" s="5"/>
-      <c r="P85" s="5"/>
-      <c r="Q85" s="5"/>
-      <c r="R85" s="5"/>
-      <c r="S85" s="5"/>
-      <c r="T85" s="5"/>
-      <c r="U85" s="5"/>
-      <c r="V85" s="5"/>
-      <c r="W85" s="6"/>
-    </row>
-    <row r="86" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B86" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E86" s="5"/>
-      <c r="F86" s="5"/>
-      <c r="G86" s="5"/>
-      <c r="H86" s="5"/>
-      <c r="I86" s="5"/>
-      <c r="J86" s="5"/>
-      <c r="K86" s="5"/>
-      <c r="L86" s="5"/>
-      <c r="M86" s="5"/>
-      <c r="N86" s="5"/>
-      <c r="O86" s="5"/>
-      <c r="P86" s="5"/>
-      <c r="Q86" s="5"/>
-      <c r="R86" s="5"/>
-      <c r="S86" s="5"/>
-      <c r="T86" s="5"/>
-      <c r="U86" s="5"/>
-      <c r="V86" s="5"/>
-      <c r="W86" s="6"/>
-    </row>
-    <row r="87" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B87" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C87" s="5"/>
-      <c r="D87" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5"/>
-      <c r="G87" s="5"/>
-      <c r="H87" s="5"/>
-      <c r="I87" s="5"/>
-      <c r="J87" s="5"/>
-      <c r="K87" s="5"/>
-      <c r="L87" s="5"/>
-      <c r="M87" s="5"/>
-      <c r="N87" s="5"/>
-      <c r="O87" s="5"/>
-      <c r="P87" s="5"/>
-      <c r="Q87" s="5"/>
-      <c r="R87" s="5"/>
-      <c r="S87" s="5"/>
-      <c r="T87" s="5"/>
-      <c r="U87" s="5"/>
-      <c r="V87" s="5"/>
-      <c r="W87" s="6"/>
-    </row>
-    <row r="88" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B88" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G88" s="5"/>
-      <c r="H88" s="5"/>
-      <c r="I88" s="5"/>
-      <c r="J88" s="5"/>
-      <c r="K88" s="5"/>
-      <c r="L88" s="5"/>
-      <c r="M88" s="5"/>
-      <c r="N88" s="5"/>
-      <c r="O88" s="5"/>
-      <c r="P88" s="5"/>
-      <c r="Q88" s="5"/>
-      <c r="R88" s="5"/>
-      <c r="S88" s="5"/>
-      <c r="T88" s="5"/>
-      <c r="U88" s="5"/>
-      <c r="V88" s="5"/>
-      <c r="W88" s="6"/>
-    </row>
-    <row r="89" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B89" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G89" s="5"/>
-      <c r="H89" s="5"/>
-      <c r="I89" s="5"/>
-      <c r="J89" s="5"/>
-      <c r="K89" s="5"/>
-      <c r="L89" s="5"/>
-      <c r="M89" s="5"/>
-      <c r="N89" s="5"/>
-      <c r="O89" s="5"/>
-      <c r="P89" s="5"/>
-      <c r="Q89" s="5"/>
-      <c r="R89" s="5"/>
-      <c r="S89" s="5"/>
-      <c r="T89" s="5"/>
-      <c r="U89" s="5"/>
-      <c r="V89" s="5"/>
-      <c r="W89" s="6"/>
-    </row>
-    <row r="90" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B90" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F90" s="5"/>
-      <c r="G90" s="5"/>
-      <c r="H90" s="5"/>
-      <c r="I90" s="5"/>
-      <c r="J90" s="5"/>
-      <c r="K90" s="5"/>
-      <c r="L90" s="5"/>
-      <c r="M90" s="5"/>
-      <c r="N90" s="5"/>
-      <c r="O90" s="5"/>
-      <c r="P90" s="5"/>
-      <c r="Q90" s="5"/>
-      <c r="R90" s="5"/>
-      <c r="S90" s="5"/>
-      <c r="T90" s="5"/>
-      <c r="U90" s="5"/>
-      <c r="V90" s="5"/>
-      <c r="W90" s="6"/>
-    </row>
-    <row r="91" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B91" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-      <c r="G91" s="5"/>
-      <c r="H91" s="5"/>
-      <c r="I91" s="5"/>
-      <c r="J91" s="5"/>
-      <c r="K91" s="5"/>
-      <c r="L91" s="5"/>
-      <c r="M91" s="5"/>
-      <c r="N91" s="5"/>
-      <c r="O91" s="5"/>
-      <c r="P91" s="5"/>
-      <c r="Q91" s="5"/>
-      <c r="R91" s="5"/>
-      <c r="S91" s="5"/>
-      <c r="T91" s="5"/>
-      <c r="U91" s="5"/>
-      <c r="V91" s="5"/>
-      <c r="W91" s="6"/>
-    </row>
-    <row r="92" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B92" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-      <c r="G92" s="5"/>
-      <c r="H92" s="5"/>
-      <c r="I92" s="5"/>
-      <c r="J92" s="5"/>
-      <c r="K92" s="5"/>
-      <c r="L92" s="5"/>
-      <c r="M92" s="5"/>
-      <c r="N92" s="5"/>
-      <c r="O92" s="5"/>
-      <c r="P92" s="5"/>
-      <c r="Q92" s="5"/>
-      <c r="R92" s="5"/>
-      <c r="S92" s="5"/>
-      <c r="T92" s="5"/>
-      <c r="U92" s="5"/>
-      <c r="V92" s="5"/>
-      <c r="W92" s="6"/>
-    </row>
-    <row r="93" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B93" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="F93" s="5"/>
-      <c r="G93" s="5"/>
-      <c r="H93" s="5"/>
-      <c r="I93" s="5"/>
-      <c r="J93" s="5"/>
-      <c r="K93" s="5"/>
-      <c r="L93" s="5"/>
-      <c r="M93" s="5"/>
-      <c r="N93" s="5"/>
-      <c r="O93" s="5"/>
-      <c r="P93" s="5"/>
-      <c r="Q93" s="5"/>
-      <c r="R93" s="5"/>
-      <c r="S93" s="5"/>
-      <c r="T93" s="5"/>
-      <c r="U93" s="5"/>
-      <c r="V93" s="5"/>
-      <c r="W93" s="6"/>
-    </row>
-    <row r="94" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B94" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F94" s="5"/>
-      <c r="G94" s="5"/>
-      <c r="H94" s="5"/>
-      <c r="I94" s="5"/>
-      <c r="J94" s="5"/>
-      <c r="K94" s="5"/>
-      <c r="L94" s="5"/>
-      <c r="M94" s="5"/>
-      <c r="N94" s="5"/>
-      <c r="O94" s="5"/>
-      <c r="P94" s="5"/>
-      <c r="Q94" s="5"/>
-      <c r="R94" s="5"/>
-      <c r="S94" s="5"/>
-      <c r="T94" s="5"/>
-      <c r="U94" s="5"/>
-      <c r="V94" s="5"/>
-      <c r="W94" s="6"/>
-    </row>
-    <row r="95" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B95" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F95" s="5"/>
-      <c r="G95" s="5"/>
-      <c r="H95" s="5"/>
-      <c r="I95" s="5"/>
-      <c r="J95" s="5"/>
-      <c r="K95" s="5"/>
-      <c r="L95" s="5"/>
-      <c r="M95" s="5"/>
-      <c r="N95" s="5"/>
-      <c r="O95" s="5"/>
-      <c r="P95" s="5"/>
-      <c r="Q95" s="5"/>
-      <c r="R95" s="5"/>
-      <c r="S95" s="5"/>
-      <c r="T95" s="5"/>
-      <c r="U95" s="5"/>
-      <c r="V95" s="5"/>
-      <c r="W95" s="6"/>
-    </row>
-    <row r="96" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B96" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
-      <c r="G96" s="5"/>
-      <c r="H96" s="5"/>
-      <c r="I96" s="5"/>
-      <c r="J96" s="5"/>
-      <c r="K96" s="5"/>
-      <c r="L96" s="5"/>
-      <c r="M96" s="5"/>
-      <c r="N96" s="5"/>
-      <c r="O96" s="5"/>
-      <c r="P96" s="5"/>
-      <c r="Q96" s="5"/>
-      <c r="R96" s="5"/>
-      <c r="S96" s="5"/>
-      <c r="T96" s="5"/>
-      <c r="U96" s="5"/>
-      <c r="V96" s="5"/>
-      <c r="W96" s="6"/>
-    </row>
-    <row r="97" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B97" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="5"/>
-      <c r="H97" s="5"/>
-      <c r="I97" s="5"/>
-      <c r="J97" s="5"/>
-      <c r="K97" s="5"/>
-      <c r="L97" s="5"/>
-      <c r="M97" s="5"/>
-      <c r="N97" s="5"/>
-      <c r="O97" s="5"/>
-      <c r="P97" s="5"/>
-      <c r="Q97" s="5"/>
-      <c r="R97" s="5"/>
-      <c r="S97" s="5"/>
-      <c r="T97" s="5"/>
-      <c r="U97" s="5"/>
-      <c r="V97" s="5"/>
-      <c r="W97" s="6"/>
-    </row>
-    <row r="98" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B98" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="5"/>
-      <c r="H98" s="5"/>
-      <c r="I98" s="5"/>
-      <c r="J98" s="5"/>
-      <c r="K98" s="5"/>
-      <c r="L98" s="5"/>
-      <c r="M98" s="5"/>
-      <c r="N98" s="5"/>
-      <c r="O98" s="5"/>
-      <c r="P98" s="5"/>
-      <c r="Q98" s="5"/>
-      <c r="R98" s="5"/>
-      <c r="S98" s="5"/>
-      <c r="T98" s="5"/>
-      <c r="U98" s="5"/>
-      <c r="V98" s="5"/>
-      <c r="W98" s="6"/>
-    </row>
-    <row r="99" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B99" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="5"/>
-      <c r="G99" s="5"/>
-      <c r="H99" s="5"/>
-      <c r="I99" s="5"/>
-      <c r="J99" s="5"/>
-      <c r="K99" s="5"/>
-      <c r="L99" s="5"/>
-      <c r="M99" s="5"/>
-      <c r="N99" s="5"/>
-      <c r="O99" s="5"/>
-      <c r="P99" s="5"/>
-      <c r="Q99" s="5"/>
-      <c r="R99" s="5"/>
-      <c r="S99" s="5"/>
-      <c r="T99" s="5"/>
-      <c r="U99" s="5"/>
-      <c r="V99" s="5"/>
-      <c r="W99" s="6"/>
-    </row>
-    <row r="100" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B100" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="5"/>
-      <c r="F100" s="5"/>
-      <c r="G100" s="5"/>
-      <c r="H100" s="5"/>
-      <c r="I100" s="5"/>
-      <c r="J100" s="5"/>
-      <c r="K100" s="5"/>
-      <c r="L100" s="5"/>
-      <c r="M100" s="5"/>
-      <c r="N100" s="5"/>
-      <c r="O100" s="5"/>
-      <c r="P100" s="5"/>
-      <c r="Q100" s="5"/>
-      <c r="R100" s="5"/>
-      <c r="S100" s="5"/>
-      <c r="T100" s="5"/>
-      <c r="U100" s="5"/>
-      <c r="V100" s="5"/>
-      <c r="W100" s="6"/>
-    </row>
-    <row r="101" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C101" s="8"/>
-      <c r="D101" s="8"/>
-      <c r="E101" s="8"/>
-      <c r="F101" s="8"/>
-      <c r="G101" s="8"/>
-      <c r="H101" s="8"/>
-      <c r="I101" s="8"/>
-      <c r="J101" s="8"/>
-      <c r="K101" s="8"/>
-      <c r="L101" s="8"/>
-      <c r="M101" s="8"/>
-      <c r="N101" s="8"/>
-      <c r="O101" s="8"/>
-      <c r="P101" s="8"/>
-      <c r="Q101" s="8"/>
-      <c r="R101" s="8"/>
-      <c r="S101" s="8"/>
-      <c r="T101" s="8"/>
-      <c r="U101" s="8"/>
-      <c r="V101" s="8"/>
-      <c r="W101" s="9"/>
+    <row r="71" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J71" s="8"/>
+      <c r="K71" s="8"/>
+      <c r="L71" s="8"/>
+      <c r="M71" s="8"/>
+      <c r="N71" s="8"/>
+      <c r="O71" s="8"/>
+      <c r="P71" s="8"/>
+      <c r="Q71" s="8"/>
+      <c r="R71" s="8"/>
+      <c r="S71" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="T71" s="8"/>
+      <c r="U71" s="8"/>
+      <c r="V71" s="8"/>
+      <c r="W71" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update entities text and diagrams
</commit_message>
<xml_diff>
--- a/Matricos.xlsx
+++ b/Matricos.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B8B8D8EB-9FA1-414C-B9D2-E10645AF46F2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="80">
   <si>
     <t>UC1</t>
   </si>
@@ -211,9 +212,6 @@
   </si>
   <si>
     <t>E11</t>
-  </si>
-  <si>
-    <t>E12</t>
   </si>
   <si>
     <t>G1</t>
@@ -267,7 +265,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -490,72 +488,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9C7957E-5114-4AC0-B33A-9427D8594DD3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8229600" y="7077075"/>
-          <a:ext cx="7553325" cy="6496050"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -820,11 +752,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:W71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="AP54" sqref="AP54"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +825,7 @@
         <v>18</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
@@ -1714,7 +1646,7 @@
       <c r="U32" s="5"/>
       <c r="V32" s="6"/>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>49</v>
       </c>
@@ -1743,9 +1675,9 @@
       <c r="U33" s="5"/>
       <c r="V33" s="6"/>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1770,7 +1702,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>50</v>
       </c>
@@ -1797,7 +1729,7 @@
       <c r="U35" s="5"/>
       <c r="V35" s="6"/>
     </row>
-    <row r="36" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="7" t="s">
         <v>51</v>
       </c>
@@ -1824,8 +1756,8 @@
       <c r="U36" s="8"/>
       <c r="V36" s="9"/>
     </row>
-    <row r="37" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="2" t="s">
         <v>53</v>
@@ -1884,14 +1816,11 @@
       <c r="U38" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="V38" s="2" t="s">
+      <c r="V38" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="W38" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
         <v>19</v>
       </c>
@@ -1916,10 +1845,9 @@
       <c r="S39" s="5"/>
       <c r="T39" s="5"/>
       <c r="U39" s="5"/>
-      <c r="V39" s="5"/>
-      <c r="W39" s="6"/>
-    </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V39" s="6"/>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
         <v>20</v>
       </c>
@@ -1937,19 +1865,18 @@
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="O40" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
       <c r="R40" s="5"/>
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
       <c r="U40" s="5"/>
-      <c r="V40" s="5"/>
-      <c r="W40" s="6"/>
-    </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V40" s="6"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B41" s="10" t="s">
         <v>21</v>
       </c>
@@ -1968,18 +1895,17 @@
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="P41" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q41" s="5"/>
       <c r="R41" s="5"/>
       <c r="S41" s="5"/>
       <c r="T41" s="5"/>
       <c r="U41" s="5"/>
-      <c r="V41" s="5"/>
-      <c r="W41" s="6"/>
-    </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V41" s="6"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="s">
         <v>22</v>
       </c>
@@ -1999,17 +1925,16 @@
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
       <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="Q42" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="R42" s="5"/>
       <c r="S42" s="5"/>
       <c r="T42" s="5"/>
       <c r="U42" s="5"/>
-      <c r="V42" s="5"/>
-      <c r="W42" s="6"/>
-    </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V42" s="6"/>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B43" s="10" t="s">
         <v>24</v>
       </c>
@@ -2030,16 +1955,15 @@
       <c r="O43" s="5"/>
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="R43" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="S43" s="5"/>
       <c r="T43" s="5"/>
       <c r="U43" s="5"/>
-      <c r="V43" s="5"/>
-      <c r="W43" s="6"/>
-    </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V43" s="6"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
         <v>25</v>
       </c>
@@ -2064,10 +1988,9 @@
       <c r="S44" s="5"/>
       <c r="T44" s="5"/>
       <c r="U44" s="5"/>
-      <c r="V44" s="5"/>
-      <c r="W44" s="6"/>
-    </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V44" s="6"/>
+    </row>
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
         <v>26</v>
       </c>
@@ -2093,13 +2016,12 @@
       <c r="R45" s="5"/>
       <c r="S45" s="5"/>
       <c r="T45" s="5"/>
-      <c r="U45" s="5"/>
-      <c r="V45" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="W45" s="6"/>
-    </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U45" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="V45" s="6"/>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B46" s="10" t="s">
         <v>27</v>
       </c>
@@ -2114,9 +2036,7 @@
       <c r="K46" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L46" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="L46" s="5"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
@@ -2125,13 +2045,12 @@
       <c r="R46" s="5"/>
       <c r="S46" s="5"/>
       <c r="T46" s="5"/>
-      <c r="U46" s="5"/>
-      <c r="V46" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="W46" s="6"/>
-    </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U46" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="V46" s="6"/>
+    </row>
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
         <v>28</v>
       </c>
@@ -2146,9 +2065,7 @@
       <c r="K47" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L47" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="L47" s="5"/>
       <c r="M47" s="5"/>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
@@ -2157,13 +2074,12 @@
       <c r="R47" s="5"/>
       <c r="S47" s="5"/>
       <c r="T47" s="5"/>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="W47" s="6"/>
-    </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U47" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="V47" s="6"/>
+    </row>
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>29</v>
       </c>
@@ -2187,13 +2103,12 @@
       <c r="R48" s="5"/>
       <c r="S48" s="5"/>
       <c r="T48" s="5"/>
-      <c r="U48" s="5"/>
-      <c r="V48" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="W48" s="6"/>
-    </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U48" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="V48" s="6"/>
+    </row>
+    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B49" s="10" t="s">
         <v>30</v>
       </c>
@@ -2216,16 +2131,15 @@
       <c r="Q49" s="5"/>
       <c r="R49" s="5"/>
       <c r="S49" s="5"/>
-      <c r="T49" s="5"/>
-      <c r="U49" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="V49" s="5"/>
-      <c r="W49" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="T49" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="U49" s="5"/>
+      <c r="V49" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
         <v>31</v>
       </c>
@@ -2240,7 +2154,9 @@
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
+      <c r="L50" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="M50" s="5"/>
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
@@ -2250,12 +2166,11 @@
       <c r="S50" s="5"/>
       <c r="T50" s="5"/>
       <c r="U50" s="5"/>
-      <c r="V50" s="5"/>
-      <c r="W50" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V50" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="s">
         <v>33</v>
       </c>
@@ -2276,9 +2191,7 @@
       <c r="M51" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="N51" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="N51" s="5"/>
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
       <c r="Q51" s="5"/>
@@ -2286,10 +2199,9 @@
       <c r="S51" s="5"/>
       <c r="T51" s="5"/>
       <c r="U51" s="5"/>
-      <c r="V51" s="5"/>
-      <c r="W51" s="6"/>
-    </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V51" s="6"/>
+    </row>
+    <row r="52" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B52" s="10" t="s">
         <v>34</v>
       </c>
@@ -2314,10 +2226,9 @@
       <c r="S52" s="5"/>
       <c r="T52" s="5"/>
       <c r="U52" s="5"/>
-      <c r="V52" s="5"/>
-      <c r="W52" s="6"/>
-    </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V52" s="6"/>
+    </row>
+    <row r="53" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B53" s="10" t="s">
         <v>35</v>
       </c>
@@ -2339,15 +2250,14 @@
       <c r="P53" s="5"/>
       <c r="Q53" s="5"/>
       <c r="R53" s="5"/>
-      <c r="S53" s="5"/>
-      <c r="T53" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="S53" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="T53" s="5"/>
       <c r="U53" s="5"/>
-      <c r="V53" s="5"/>
-      <c r="W53" s="6"/>
-    </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V53" s="6"/>
+    </row>
+    <row r="54" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="s">
         <v>36</v>
       </c>
@@ -2362,7 +2272,9 @@
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
+      <c r="L54" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="M54" s="5"/>
       <c r="N54" s="5"/>
       <c r="O54" s="5"/>
@@ -2370,16 +2282,15 @@
       <c r="Q54" s="5"/>
       <c r="R54" s="5"/>
       <c r="S54" s="5"/>
-      <c r="T54" s="5"/>
-      <c r="U54" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="V54" s="5"/>
-      <c r="W54" s="6"/>
-    </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="T54" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="U54" s="5"/>
+      <c r="V54" s="6"/>
+    </row>
+    <row r="55" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B55" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>52</v>
@@ -2394,20 +2305,19 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
       <c r="M55" s="5"/>
-      <c r="N55" s="5"/>
-      <c r="O55" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="N55" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="O55" s="5"/>
       <c r="P55" s="5"/>
       <c r="Q55" s="5"/>
       <c r="R55" s="5"/>
       <c r="S55" s="5"/>
       <c r="T55" s="5"/>
       <c r="U55" s="5"/>
-      <c r="V55" s="5"/>
-      <c r="W55" s="6"/>
-    </row>
-    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V55" s="6"/>
+    </row>
+    <row r="56" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
         <v>38</v>
       </c>
@@ -2432,10 +2342,9 @@
       <c r="S56" s="5"/>
       <c r="T56" s="5"/>
       <c r="U56" s="5"/>
-      <c r="V56" s="5"/>
-      <c r="W56" s="6"/>
-    </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V56" s="6"/>
+    </row>
+    <row r="57" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>39</v>
       </c>
@@ -2450,7 +2359,9 @@
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
-      <c r="L57" s="5"/>
+      <c r="L57" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="M57" s="5"/>
       <c r="N57" s="5"/>
       <c r="O57" s="5"/>
@@ -2460,10 +2371,9 @@
       <c r="S57" s="5"/>
       <c r="T57" s="5"/>
       <c r="U57" s="5"/>
-      <c r="V57" s="5"/>
-      <c r="W57" s="6"/>
-    </row>
-    <row r="58" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V57" s="6"/>
+    </row>
+    <row r="58" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>40</v>
       </c>
@@ -2490,10 +2400,9 @@
       <c r="S58" s="5"/>
       <c r="T58" s="5"/>
       <c r="U58" s="5"/>
-      <c r="V58" s="5"/>
-      <c r="W58" s="6"/>
-    </row>
-    <row r="59" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V58" s="6"/>
+    </row>
+    <row r="59" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>41</v>
       </c>
@@ -2518,10 +2427,9 @@
       <c r="S59" s="5"/>
       <c r="T59" s="5"/>
       <c r="U59" s="5"/>
-      <c r="V59" s="5"/>
-      <c r="W59" s="6"/>
-    </row>
-    <row r="60" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V59" s="6"/>
+    </row>
+    <row r="60" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>42</v>
       </c>
@@ -2546,10 +2454,9 @@
       <c r="S60" s="5"/>
       <c r="T60" s="5"/>
       <c r="U60" s="5"/>
-      <c r="V60" s="5"/>
-      <c r="W60" s="6"/>
-    </row>
-    <row r="61" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V60" s="6"/>
+    </row>
+    <row r="61" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B61" s="10" t="s">
         <v>43</v>
       </c>
@@ -2574,10 +2481,9 @@
       <c r="S61" s="5"/>
       <c r="T61" s="5"/>
       <c r="U61" s="5"/>
-      <c r="V61" s="5"/>
-      <c r="W61" s="6"/>
-    </row>
-    <row r="62" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V61" s="6"/>
+    </row>
+    <row r="62" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B62" s="10" t="s">
         <v>44</v>
       </c>
@@ -2595,19 +2501,18 @@
       <c r="L62" s="5"/>
       <c r="M62" s="5"/>
       <c r="N62" s="5"/>
-      <c r="O62" s="5"/>
-      <c r="P62" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="O62" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="P62" s="5"/>
       <c r="Q62" s="5"/>
       <c r="R62" s="5"/>
       <c r="S62" s="5"/>
       <c r="T62" s="5"/>
       <c r="U62" s="5"/>
-      <c r="V62" s="5"/>
-      <c r="W62" s="6"/>
-    </row>
-    <row r="63" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V62" s="6"/>
+    </row>
+    <row r="63" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B63" s="10" t="s">
         <v>45</v>
       </c>
@@ -2625,19 +2530,18 @@
       <c r="L63" s="5"/>
       <c r="M63" s="5"/>
       <c r="N63" s="5"/>
-      <c r="O63" s="5"/>
-      <c r="P63" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="O63" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="P63" s="5"/>
       <c r="Q63" s="5"/>
       <c r="R63" s="5"/>
       <c r="S63" s="5"/>
       <c r="T63" s="5"/>
       <c r="U63" s="5"/>
-      <c r="V63" s="5"/>
-      <c r="W63" s="6"/>
-    </row>
-    <row r="64" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V63" s="6"/>
+    </row>
+    <row r="64" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B64" s="10" t="s">
         <v>46</v>
       </c>
@@ -2665,13 +2569,12 @@
       <c r="R64" s="5"/>
       <c r="S64" s="5"/>
       <c r="T64" s="5"/>
-      <c r="U64" s="5"/>
-      <c r="V64" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="W64" s="6"/>
-    </row>
-    <row r="65" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U64" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="V64" s="6"/>
+    </row>
+    <row r="65" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B65" s="10" t="s">
         <v>47</v>
       </c>
@@ -2686,9 +2589,7 @@
       <c r="K65" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L65" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="L65" s="5"/>
       <c r="M65" s="5"/>
       <c r="N65" s="5"/>
       <c r="O65" s="5"/>
@@ -2698,10 +2599,9 @@
       <c r="S65" s="5"/>
       <c r="T65" s="5"/>
       <c r="U65" s="5"/>
-      <c r="V65" s="5"/>
-      <c r="W65" s="6"/>
-    </row>
-    <row r="66" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V65" s="6"/>
+    </row>
+    <row r="66" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
         <v>48</v>
       </c>
@@ -2716,9 +2616,7 @@
       <c r="K66" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L66" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="L66" s="5"/>
       <c r="M66" s="5"/>
       <c r="N66" s="5"/>
       <c r="O66" s="5"/>
@@ -2728,10 +2626,9 @@
       <c r="S66" s="5"/>
       <c r="T66" s="5"/>
       <c r="U66" s="5"/>
-      <c r="V66" s="5"/>
-      <c r="W66" s="6"/>
-    </row>
-    <row r="67" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V66" s="6"/>
+    </row>
+    <row r="67" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B67" s="10" t="s">
         <v>49</v>
       </c>
@@ -2746,9 +2643,7 @@
       <c r="K67" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L67" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="L67" s="5"/>
       <c r="M67" s="5"/>
       <c r="N67" s="5"/>
       <c r="O67" s="5"/>
@@ -2758,12 +2653,11 @@
       <c r="S67" s="5"/>
       <c r="T67" s="5"/>
       <c r="U67" s="5"/>
-      <c r="V67" s="5"/>
-      <c r="W67" s="6"/>
-    </row>
-    <row r="68" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V67" s="6"/>
+    </row>
+    <row r="68" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B68" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -2786,12 +2680,11 @@
       <c r="S68" s="5"/>
       <c r="T68" s="5"/>
       <c r="U68" s="5"/>
-      <c r="V68" s="5"/>
-      <c r="W68" s="6"/>
-    </row>
-    <row r="69" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V68" s="6"/>
+    </row>
+    <row r="69" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B69" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -2814,12 +2707,11 @@
       <c r="S69" s="5"/>
       <c r="T69" s="5"/>
       <c r="U69" s="5"/>
-      <c r="V69" s="5"/>
-      <c r="W69" s="6"/>
-    </row>
-    <row r="70" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V69" s="6"/>
+    </row>
+    <row r="70" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B70" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -2838,18 +2730,17 @@
       <c r="O70" s="5"/>
       <c r="P70" s="5"/>
       <c r="Q70" s="5"/>
-      <c r="R70" s="5"/>
-      <c r="S70" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="R70" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="S70" s="5"/>
       <c r="T70" s="5"/>
       <c r="U70" s="5"/>
-      <c r="V70" s="5"/>
-      <c r="W70" s="6"/>
-    </row>
-    <row r="71" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V70" s="6"/>
+    </row>
+    <row r="71" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
@@ -2868,18 +2759,16 @@
       <c r="O71" s="8"/>
       <c r="P71" s="8"/>
       <c r="Q71" s="8"/>
-      <c r="R71" s="8"/>
-      <c r="S71" s="8" t="s">
-        <v>52</v>
-      </c>
+      <c r="R71" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="S71" s="8"/>
       <c r="T71" s="8"/>
       <c r="U71" s="8"/>
-      <c r="V71" s="8"/>
-      <c r="W71" s="9"/>
+      <c r="V71" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>